<commit_message>
Add automatic detection and sample measurement data
</commit_message>
<xml_diff>
--- a/WorkingData/SteadyCalibrationCurve.xlsx
+++ b/WorkingData/SteadyCalibrationCurve.xlsx
@@ -793,148 +793,148 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>160</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>240</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>320</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>400</c:v>
+                  <c:v>375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>480</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>560</c:v>
+                  <c:v>525</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>640</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>720</c:v>
+                  <c:v>675</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>800</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>880</c:v>
+                  <c:v>825</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>960</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1040</c:v>
+                  <c:v>975</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1120</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>1280</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>1360</c:v>
+                  <c:v>1275</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1440</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1520</c:v>
+                  <c:v>1425</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1600</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1680</c:v>
+                  <c:v>1575</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1760</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1840</c:v>
+                  <c:v>1725</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1920</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2000</c:v>
+                  <c:v>1875</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2080</c:v>
+                  <c:v>1950</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2160</c:v>
+                  <c:v>2025</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2240</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2320</c:v>
+                  <c:v>2175</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2325</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>2400</c:v>
                 </c:pt>
-                <c:pt idx="31">
-                  <c:v>2480</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2560</c:v>
-                </c:pt>
                 <c:pt idx="33">
-                  <c:v>2640</c:v>
+                  <c:v>2475</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2720</c:v>
+                  <c:v>2550</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2800</c:v>
+                  <c:v>2625</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2880</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2960</c:v>
+                  <c:v>2775</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3040</c:v>
+                  <c:v>2850</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3120</c:v>
+                  <c:v>2925</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3200</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3280</c:v>
+                  <c:v>3075</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3360</c:v>
+                  <c:v>3150</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3440</c:v>
+                  <c:v>3225</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3520</c:v>
+                  <c:v>3300</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>3375</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3450</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3525</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3680</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3760</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>3840</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3343,8 +3343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B2">
         <v>580.32799999999997</v>
@@ -3373,7 +3373,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B3">
         <v>538.32799999999997</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B4">
         <v>640.32799999999997</v>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="B5">
         <v>611.32799999999997</v>
@@ -3406,7 +3406,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>400</v>
+        <v>375</v>
       </c>
       <c r="B6">
         <v>551.32799999999997</v>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>480</v>
+        <v>450</v>
       </c>
       <c r="B7">
         <v>563.32799999999997</v>
@@ -3428,7 +3428,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>560</v>
+        <v>525</v>
       </c>
       <c r="B8">
         <v>676.32799999999997</v>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="B9">
         <v>621.32799999999997</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>720</v>
+        <v>675</v>
       </c>
       <c r="B10">
         <v>576.32799999999997</v>
@@ -3461,7 +3461,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="B11">
         <v>633.32799999999997</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>880</v>
+        <v>825</v>
       </c>
       <c r="B12">
         <v>596.32799999999997</v>
@@ -3483,7 +3483,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>960</v>
+        <v>900</v>
       </c>
       <c r="B13">
         <v>627.32799999999997</v>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1040</v>
+        <v>975</v>
       </c>
       <c r="B14">
         <v>627.32799999999997</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>1120</v>
+        <v>1050</v>
       </c>
       <c r="B15">
         <v>602.32799999999997</v>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1200</v>
+        <v>1125</v>
       </c>
       <c r="B16">
         <v>643.32799999999997</v>
@@ -3527,7 +3527,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>1280</v>
+        <v>1200</v>
       </c>
       <c r="B17">
         <v>642.32799999999997</v>
@@ -3538,7 +3538,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>1360</v>
+        <v>1275</v>
       </c>
       <c r="B18">
         <v>573.32799999999997</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>1440</v>
+        <v>1350</v>
       </c>
       <c r="B19">
         <v>521.32799999999997</v>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>1520</v>
+        <v>1425</v>
       </c>
       <c r="B20">
         <v>548.32799999999997</v>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="B21">
         <v>563.32799999999997</v>
@@ -3582,7 +3582,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>1680</v>
+        <v>1575</v>
       </c>
       <c r="B22">
         <v>581.32799999999997</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>1760</v>
+        <v>1650</v>
       </c>
       <c r="B23">
         <v>576.32799999999997</v>
@@ -3604,7 +3604,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>1840</v>
+        <v>1725</v>
       </c>
       <c r="B24">
         <v>3063.33</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>1920</v>
+        <v>1800</v>
       </c>
       <c r="B25">
         <v>22804.3</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>2000</v>
+        <v>1875</v>
       </c>
       <c r="B26">
         <v>43545.3</v>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>2080</v>
+        <v>1950</v>
       </c>
       <c r="B27">
         <v>45726.3</v>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>2160</v>
+        <v>2025</v>
       </c>
       <c r="B28">
         <v>45599.3</v>
@@ -3659,7 +3659,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>2240</v>
+        <v>2100</v>
       </c>
       <c r="B29">
         <v>45712.3</v>
@@ -3670,7 +3670,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>2320</v>
+        <v>2175</v>
       </c>
       <c r="B30">
         <v>45648.3</v>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>2400</v>
+        <v>2250</v>
       </c>
       <c r="B31">
         <v>45661.3</v>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>2480</v>
+        <v>2325</v>
       </c>
       <c r="B32">
         <v>45644.3</v>
@@ -3703,7 +3703,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>2560</v>
+        <v>2400</v>
       </c>
       <c r="B33">
         <v>47586.3</v>
@@ -3714,7 +3714,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>2640</v>
+        <v>2475</v>
       </c>
       <c r="B34">
         <v>49550.3</v>
@@ -3725,7 +3725,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>2720</v>
+        <v>2550</v>
       </c>
       <c r="B35">
         <v>46800.3</v>
@@ -3736,7 +3736,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>2800</v>
+        <v>2625</v>
       </c>
       <c r="B36">
         <v>47595.3</v>
@@ -3747,7 +3747,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>2880</v>
+        <v>2700</v>
       </c>
       <c r="B37">
         <v>45127.3</v>
@@ -3758,7 +3758,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>2960</v>
+        <v>2775</v>
       </c>
       <c r="B38">
         <v>17227.3</v>
@@ -3769,7 +3769,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>3040</v>
+        <v>2850</v>
       </c>
       <c r="B39">
         <v>1009.33</v>
@@ -3780,7 +3780,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>3120</v>
+        <v>2925</v>
       </c>
       <c r="B40">
         <v>420.32799999999997</v>
@@ -3791,7 +3791,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>3200</v>
+        <v>3000</v>
       </c>
       <c r="B41">
         <v>467.32799999999997</v>
@@ -3802,7 +3802,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>3280</v>
+        <v>3075</v>
       </c>
       <c r="B42">
         <v>439.32799999999997</v>
@@ -3813,7 +3813,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>3360</v>
+        <v>3150</v>
       </c>
       <c r="B43">
         <v>425.32799999999997</v>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>3440</v>
+        <v>3225</v>
       </c>
       <c r="B44">
         <v>459.32799999999997</v>
@@ -3835,7 +3835,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>3520</v>
+        <v>3300</v>
       </c>
       <c r="B45">
         <v>419.32799999999997</v>
@@ -3846,7 +3846,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>3600</v>
+        <v>3375</v>
       </c>
       <c r="B46">
         <v>400.32799999999997</v>
@@ -3857,7 +3857,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>3680</v>
+        <v>3450</v>
       </c>
       <c r="B47">
         <v>482.32799999999997</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>3760</v>
+        <v>3525</v>
       </c>
       <c r="B48">
         <v>442.32799999999997</v>
@@ -3879,7 +3879,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>3840</v>
+        <v>3600</v>
       </c>
       <c r="B49">
         <v>429.32799999999997</v>

</xml_diff>